<commit_message>
Atualização da planilha URIs_e_BD.xlsx
Atualização da planilha URIs_e_BD.xlsx. Ajuste na explicação do caminho dos arquivos de dump.
</commit_message>
<xml_diff>
--- a/doc/URIs_e_BD.xlsx
+++ b/doc/URIs_e_BD.xlsx
@@ -14,24 +14,39 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
+    <t>Instruções de restauração do Banco de dados SWChallenge</t>
+  </si>
+  <si>
     <t>Método/Verbo Http</t>
   </si>
   <si>
-    <t>Instruções de restauração do Banco de dados SWChallenge</t>
+    <t>1º</t>
   </si>
   <si>
     <t>URL</t>
   </si>
   <si>
+    <t>Acessar a pasta bin no caminho de instalação do MongoDB</t>
+  </si>
+  <si>
+    <t>2º</t>
+  </si>
+  <si>
+    <t>Caso não exista, criar a pasta "dump"</t>
+  </si>
+  <si>
+    <t>3º</t>
+  </si>
+  <si>
     <t>Parâmetros</t>
   </si>
   <si>
-    <t>1º</t>
-  </si>
-  <si>
     <t>Descrição do método</t>
   </si>
   <si>
+    <t>Copiar para a pasta dump do MongoDB o conteúdo da pasta "dump\SWChallenge" do projeto (todos os arquivos .bson e .json)</t>
+  </si>
+  <si>
     <t>Post</t>
   </si>
   <si>
@@ -74,6 +89,9 @@
     <t>Busca uma lista com todos os Planetas cadastrados na aplicação</t>
   </si>
   <si>
+    <t>4º</t>
+  </si>
+  <si>
     <t>Delete</t>
   </si>
   <si>
@@ -81,24 +99,6 @@
   </si>
   <si>
     <t>Remove o registro de um planeta cadastrado na aplicação</t>
-  </si>
-  <si>
-    <t>Acessar a pasta bin no caminho de instalação do MongoDB</t>
-  </si>
-  <si>
-    <t>2º</t>
-  </si>
-  <si>
-    <t>Caso não exista, criar a pasta "dump"</t>
-  </si>
-  <si>
-    <t>3º</t>
-  </si>
-  <si>
-    <t>Copiar para a pasta dump do MongoDB o conteúdo da pasta dump do projeto swchallenge(todos os arquivos .bson e .json)</t>
-  </si>
-  <si>
-    <t>4º</t>
   </si>
   <si>
     <t>Abrir um promp como administrador</t>
@@ -141,10 +141,10 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <b/>
     </font>
+    <font/>
   </fonts>
   <fills count="4">
     <fill>
@@ -177,17 +177,17 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -224,87 +224,87 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1"/>
@@ -1315,37 +1315,37 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>24</v>
+      <c r="A3" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>26</v>
+      <c r="A4" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>

</xml_diff>